<commit_message>
redmine #9139 cal sheets for  CP04OSPM multiple deployments added/changed.
</commit_message>
<xml_diff>
--- a/CP04OSPM/Omaha_Cal_Info_CP04OSPM_00002.xlsx
+++ b/CP04OSPM/Omaha_Cal_Info_CP04OSPM_00002.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Documents\Project Info\WHOI\Marine Integration - OOI\OOInet Migration\Integration\Cal and Ingest Sheets\Sheets from -test 2015-08-19\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="14052" windowHeight="5580" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="10200" yWindow="10180" windowWidth="24640" windowHeight="9800" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -23,24 +18,29 @@
     <definedName name="_FilterDatabase_0_0_0">Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0_0">Moorings!$A$1:$J$83</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$397</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$398</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$397</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_1">Asset_Cal_Info!$A$1:$F$397</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0">Asset_Cal_Info!$A$1:$F$398</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_1">Asset_Cal_Info!$A$1:$F$398</definedName>
     <definedName name="_FilterDatabase_0_0_0_1">Asset_Cal_Info!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_1">Asset_Cal_Info!$A$1:$F$397</definedName>
+    <definedName name="_FilterDatabase_0_0_1">Asset_Cal_Info!$A$1:$F$398</definedName>
     <definedName name="_FilterDatabase_0_1">Asset_Cal_Info!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_1">Asset_Cal_Info!$A$1:$F$29</definedName>
     <definedName name="_FilterDatabase_1_1">Asset_Cal_Info!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$83</definedName>
-    <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$397</definedName>
+    <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$398</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
   <si>
     <t>Ref Des</t>
   </si>
@@ -227,9 +227,6 @@
     <t>Located in the calibration certificate for QSP-2200, under Calibration Factors, after Wet (Volts/(quanta/cm2-sec))</t>
   </si>
   <si>
-    <t>KN 222</t>
-  </si>
-  <si>
     <t>39° 56.491' N</t>
   </si>
   <si>
@@ -239,25 +236,13 @@
     <t>This serial number is a placekeeper used until the correct serial number is found or defined</t>
   </si>
   <si>
-    <t>CP04OSPM-SBS01-00-RTE000000</t>
-  </si>
-  <si>
     <t>CP04OSPM-WFP01-00-WFPENG000</t>
   </si>
   <si>
     <t>CP04OSPM-SBS01-01-MOPAK0000</t>
   </si>
   <si>
-    <t>OSPM-00002-RTE</t>
-  </si>
-  <si>
-    <t>OSPM-00002-STC</t>
-  </si>
-  <si>
     <t>OSPM-00002-MOPAK</t>
-  </si>
-  <si>
-    <t>OSPM-00002-WFP</t>
   </si>
   <si>
     <t>CC_angular_resolution</t>
@@ -296,6 +281,15 @@
       <t>-VEL3DK000</t>
     </r>
   </si>
+  <si>
+    <t>KN-222</t>
+  </si>
+  <si>
+    <t>12936-01</t>
+  </si>
+  <si>
+    <t>SWE 0012</t>
+  </si>
 </sst>
 </file>
 
@@ -304,7 +298,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -397,8 +391,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -409,6 +436,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCECFF"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -475,11 +508,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -543,9 +592,43 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="18">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -672,7 +755,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -707,7 +790,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -918,28 +1001,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="F2" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.88671875"/>
-    <col min="2" max="2" width="39.44140625"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.44140625"/>
-    <col min="7" max="7" width="18.6640625"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875"/>
-    <col min="10" max="10" width="12.6640625"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="10" width="11.1640625" customWidth="1"/>
     <col min="11" max="11" width="44" customWidth="1"/>
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="1026" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.2">
+    <row r="1" spans="1:13" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -955,7 +1033,7 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="29" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -990,28 +1068,24 @@
       <c r="E2" s="12">
         <v>0.83611111111111114</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="30">
+        <v>42123</v>
+      </c>
       <c r="G2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="5">
-        <v>455</v>
+      <c r="I2" s="27">
+        <v>450</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="K2" s="6"/>
-      <c r="L2" s="15">
-        <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
-        <v>39.941516666666665</v>
-      </c>
-      <c r="M2" s="15">
-        <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
-        <v>-70.878433333333334</v>
-      </c>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13">
       <c r="D3" s="9"/>
@@ -1023,35 +1097,35 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.33203125" customWidth="1"/>
     <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625"/>
-    <col min="9" max="9" width="11.88671875"/>
-    <col min="10" max="10" width="14.44140625"/>
-    <col min="11" max="11" width="13.44140625"/>
-    <col min="12" max="1026" width="8.6640625"/>
+    <col min="5" max="5" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6">
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1325,7 +1399,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>40</v>
@@ -1347,7 +1421,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>40</v>
@@ -1391,10 +1465,10 @@
         <v>969</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="20">
-        <v>1.08</v>
+        <v>60</v>
+      </c>
+      <c r="F17" s="25">
+        <v>1.0760000000000001</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>33</v>
@@ -1487,9 +1561,9 @@
         <v>969</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" s="20">
+        <v>61</v>
+      </c>
+      <c r="F21" s="26">
         <v>3.9E-2</v>
       </c>
       <c r="G21" s="17" t="s">
@@ -1511,9 +1585,9 @@
         <v>969</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="20">
+        <v>62</v>
+      </c>
+      <c r="F22" s="26">
         <v>700</v>
       </c>
       <c r="G22" s="17" t="s">
@@ -1607,10 +1681,10 @@
         <v>969</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="F26" s="20">
-        <v>117</v>
+        <v>63</v>
+      </c>
+      <c r="F26" s="25">
+        <v>124</v>
       </c>
       <c r="G26" s="17" t="s">
         <v>33</v>
@@ -1687,7 +1761,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="16" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="B31" s="17" t="s">
         <v>40</v>
@@ -1695,81 +1769,84 @@
       <c r="C31" s="17">
         <v>2</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>62</v>
+      <c r="D31" s="28" t="s">
+        <v>66</v>
       </c>
       <c r="E31" s="16"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="24" t="s">
-        <v>57</v>
-      </c>
+      <c r="F31" s="16"/>
+      <c r="G31" s="24"/>
       <c r="H31" s="16"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="17">
-        <v>2</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>61</v>
-      </c>
+      <c r="A32" s="16"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="23"/>
       <c r="E32" s="16"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="24" t="s">
-        <v>57</v>
-      </c>
+      <c r="F32" s="16"/>
+      <c r="G32" s="24"/>
       <c r="H32" s="16"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="17">
+        <v>2</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="16"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="H33" s="16"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="16"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="16"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="17">
+        <v>2</v>
+      </c>
+      <c r="D35" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="17">
-        <v>2</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="H33" s="16"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="17">
-        <v>2</v>
-      </c>
-      <c r="D34" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="H34" s="16"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="8"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="H35" s="16"/>
+    </row>
+    <row r="36" spans="1:8" ht="15">
+      <c r="A36" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>